<commit_message>
HUfflepuff + Ravenclaw (almost) done
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Archetypes/Empath.xlsx
+++ b/CoreRulebook/Data/Archetypes/Empath.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">LVL</t>
   </si>
   <si>
     <t xml:space="preserve">Arcane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empath</t>
   </si>
   <si>
     <t xml:space="preserve">Seer</t>
@@ -189,17 +192,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B21"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="41.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,6 +218,9 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -225,7 +231,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,7 +243,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,11 +254,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A4/5)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,11 +269,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A5/5)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,11 +284,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A6/5)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,11 +299,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A7/5)</f>
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,8 +314,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A8/5)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>13</v>
+      <c r="E8" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,11 +326,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A9/5)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,8 +341,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A10/5)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>15</v>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,8 +353,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A11/5)</f>
         <v>2</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>16</v>
+      <c r="E11" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,8 +365,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A12/5)</f>
         <v>2</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,8 +377,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A13/5)</f>
         <v>2</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>18</v>
+      <c r="E13" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,11 +389,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A14/5)</f>
         <v>2</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,8 +413,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A16/5)</f>
         <v>3</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>20</v>
+      <c r="E16" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,8 +425,8 @@
         <f aca="false">_xlfn.FLOOR.MATH(A17/5)</f>
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,11 +446,11 @@
         <f aca="false">_xlfn.FLOOR.MATH(A19/5)</f>
         <v>3</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="D19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>